<commit_message>
all data imported to data frames with datetime
</commit_message>
<xml_diff>
--- a/population growht.xlsx
+++ b/population growht.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EE6C5A5-718A-4B71-9346-D33E8A7992B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clarissaseebohm/Desktop/Save-The-GSL/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A25FE10-B803-FF4A-B13B-247A65395D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11040" yWindow="2840" windowWidth="20060" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +48,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -389,1372 +394,1372 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:E126"/>
+  <dimension ref="A1:C124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection sqref="A1:C124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="3:5">
-      <c r="C3" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="3:5">
-      <c r="C4" s="1">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>336</v>
       </c>
-      <c r="D4">
+      <c r="B2">
         <v>277000</v>
       </c>
     </row>
-    <row r="5" spans="3:5">
-      <c r="C5" s="1">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>701</v>
       </c>
-      <c r="D5">
+      <c r="B3">
         <v>284000</v>
       </c>
-      <c r="E5">
+      <c r="C3">
         <v>2.5299999999999998</v>
       </c>
     </row>
-    <row r="6" spans="3:5">
-      <c r="C6" s="1">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>1066</v>
       </c>
-      <c r="D6">
+      <c r="B4">
         <v>292000</v>
       </c>
-      <c r="E6">
+      <c r="C4">
         <v>2.82</v>
       </c>
     </row>
-    <row r="7" spans="3:5">
-      <c r="C7" s="1">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>1431</v>
       </c>
-      <c r="D7">
+      <c r="B5">
         <v>299000</v>
       </c>
-      <c r="E7">
+      <c r="C5">
         <v>2.4</v>
       </c>
     </row>
-    <row r="8" spans="3:5">
-      <c r="C8" s="1">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>1797</v>
       </c>
-      <c r="D8">
+      <c r="B6">
         <v>308000</v>
       </c>
-      <c r="E8">
+      <c r="C6">
         <v>3.01</v>
       </c>
     </row>
-    <row r="9" spans="3:5">
-      <c r="C9" s="1">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>2162</v>
       </c>
-      <c r="D9">
+      <c r="B7">
         <v>316000</v>
       </c>
-      <c r="E9">
+      <c r="C7">
         <v>2.6</v>
       </c>
     </row>
-    <row r="10" spans="3:5">
-      <c r="C10" s="1">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>2527</v>
       </c>
-      <c r="D10">
+      <c r="B8">
         <v>327000</v>
       </c>
-      <c r="E10">
+      <c r="C8">
         <v>3.48</v>
       </c>
     </row>
-    <row r="11" spans="3:5">
-      <c r="C11" s="1">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>2892</v>
       </c>
-      <c r="D11">
+      <c r="B9">
         <v>339000</v>
       </c>
-      <c r="E11">
+      <c r="C9">
         <v>3.67</v>
       </c>
     </row>
-    <row r="12" spans="3:5">
-      <c r="C12" s="1">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>3258</v>
       </c>
-      <c r="D12">
+      <c r="B10">
         <v>351000</v>
       </c>
-      <c r="E12">
+      <c r="C10">
         <v>3.54</v>
       </c>
     </row>
-    <row r="13" spans="3:5">
-      <c r="C13" s="1">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>3623</v>
       </c>
-      <c r="D13">
+      <c r="B11">
         <v>363000</v>
       </c>
-      <c r="E13">
+      <c r="C11">
         <v>3.42</v>
       </c>
     </row>
-    <row r="14" spans="3:5">
-      <c r="C14" s="1">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>3988</v>
       </c>
-      <c r="D14">
+      <c r="B12">
         <v>377000</v>
       </c>
-      <c r="E14">
+      <c r="C12">
         <v>3.86</v>
       </c>
     </row>
-    <row r="15" spans="3:5">
-      <c r="C15" s="1">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>4353</v>
       </c>
-      <c r="D15">
+      <c r="B13">
         <v>387000</v>
       </c>
-      <c r="E15">
+      <c r="C13">
         <v>2.65</v>
       </c>
     </row>
-    <row r="16" spans="3:5">
-      <c r="C16" s="1">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
         <v>4719</v>
       </c>
-      <c r="D16">
+      <c r="B14">
         <v>399000</v>
       </c>
-      <c r="E16">
+      <c r="C14">
         <v>3.1</v>
       </c>
     </row>
-    <row r="17" spans="3:5">
-      <c r="C17" s="1">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>5084</v>
       </c>
-      <c r="D17">
+      <c r="B15">
         <v>410000</v>
       </c>
-      <c r="E17">
+      <c r="C15">
         <v>2.76</v>
       </c>
     </row>
-    <row r="18" spans="3:5">
-      <c r="C18" s="1">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
         <v>5449</v>
       </c>
-      <c r="D18">
+      <c r="B16">
         <v>422000</v>
       </c>
-      <c r="E18">
+      <c r="C16">
         <v>2.93</v>
       </c>
     </row>
-    <row r="19" spans="3:5">
-      <c r="C19" s="1">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
         <v>5814</v>
       </c>
-      <c r="D19">
+      <c r="B17">
         <v>430000</v>
       </c>
-      <c r="E19">
+      <c r="C17">
         <v>1.9</v>
       </c>
     </row>
-    <row r="20" spans="3:5">
-      <c r="C20" s="1">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
         <v>6180</v>
       </c>
-      <c r="D20">
+      <c r="B18">
         <v>436000</v>
       </c>
-      <c r="E20">
+      <c r="C18">
         <v>1.4</v>
       </c>
     </row>
-    <row r="21" spans="3:5">
-      <c r="C21" s="1">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
         <v>6545</v>
       </c>
-      <c r="D21">
+      <c r="B19">
         <v>444000</v>
       </c>
-      <c r="E21">
+      <c r="C19">
         <v>1.83</v>
       </c>
     </row>
-    <row r="22" spans="3:5">
-      <c r="C22" s="1">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
         <v>6910</v>
       </c>
-      <c r="D22">
+      <c r="B20">
         <v>437000</v>
       </c>
-      <c r="E22">
+      <c r="C20">
         <v>-1.58</v>
       </c>
     </row>
-    <row r="23" spans="3:5">
-      <c r="C23" s="1">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
         <v>7275</v>
       </c>
-      <c r="D23">
+      <c r="B21">
         <v>446000</v>
       </c>
-      <c r="E23">
+      <c r="C21">
         <v>2.06</v>
       </c>
     </row>
-    <row r="24" spans="3:5">
-      <c r="C24" s="1">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
         <v>7641</v>
       </c>
-      <c r="D24">
+      <c r="B22">
         <v>453000</v>
       </c>
-      <c r="E24">
+      <c r="C22">
         <v>1.57</v>
       </c>
     </row>
-    <row r="25" spans="3:5">
-      <c r="C25" s="1">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
         <v>8006</v>
       </c>
-      <c r="D25">
+      <c r="B23">
         <v>457000</v>
       </c>
-      <c r="E25">
+      <c r="C23">
         <v>0.88</v>
       </c>
     </row>
-    <row r="26" spans="3:5">
-      <c r="C26" s="1">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
         <v>8371</v>
       </c>
-      <c r="D26">
+      <c r="B24">
         <v>467000</v>
       </c>
-      <c r="E26">
+      <c r="C24">
         <v>2.19</v>
       </c>
     </row>
-    <row r="27" spans="3:5">
-      <c r="C27" s="1">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
         <v>8736</v>
       </c>
-      <c r="D27">
+      <c r="B25">
         <v>474000</v>
       </c>
-      <c r="E27">
+      <c r="C25">
         <v>1.5</v>
       </c>
     </row>
-    <row r="28" spans="3:5">
-      <c r="C28" s="1">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
         <v>9102</v>
       </c>
-      <c r="D28">
+      <c r="B26">
         <v>481000</v>
       </c>
-      <c r="E28">
+      <c r="C26">
         <v>1.48</v>
       </c>
     </row>
-    <row r="29" spans="3:5">
-      <c r="C29" s="1">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
         <v>9467</v>
       </c>
-      <c r="D29">
+      <c r="B27">
         <v>487000</v>
       </c>
-      <c r="E29">
+      <c r="C27">
         <v>1.25</v>
       </c>
     </row>
-    <row r="30" spans="3:5">
-      <c r="C30" s="1">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
         <v>9832</v>
       </c>
-      <c r="D30">
+      <c r="B28">
         <v>494000</v>
       </c>
-      <c r="E30">
+      <c r="C28">
         <v>1.44</v>
       </c>
     </row>
-    <row r="31" spans="3:5">
-      <c r="C31" s="1">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
         <v>10197</v>
       </c>
-      <c r="D31">
+      <c r="B29">
         <v>500000</v>
       </c>
-      <c r="E31">
+      <c r="C29">
         <v>1.21</v>
       </c>
     </row>
-    <row r="32" spans="3:5">
-      <c r="C32" s="1">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
         <v>10563</v>
       </c>
-      <c r="D32">
+      <c r="B30">
         <v>504000</v>
       </c>
-      <c r="E32">
+      <c r="C30">
         <v>0.8</v>
       </c>
     </row>
-    <row r="33" spans="3:5">
-      <c r="C33" s="1">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
         <v>10928</v>
       </c>
-      <c r="D33">
+      <c r="B31">
         <v>508000</v>
       </c>
-      <c r="E33">
+      <c r="C31">
         <v>0.79</v>
       </c>
     </row>
-    <row r="34" spans="3:5">
-      <c r="C34" s="1">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
         <v>11293</v>
       </c>
-      <c r="D34">
+      <c r="B32">
         <v>509000</v>
       </c>
-      <c r="E34">
+      <c r="C32">
         <v>0.2</v>
       </c>
     </row>
-    <row r="35" spans="3:5">
-      <c r="C35" s="1">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
         <v>11658</v>
       </c>
-      <c r="D35">
+      <c r="B33">
         <v>513000</v>
       </c>
-      <c r="E35">
+      <c r="C33">
         <v>0.79</v>
       </c>
     </row>
-    <row r="36" spans="3:5">
-      <c r="C36" s="1">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
         <v>12024</v>
       </c>
-      <c r="D36">
+      <c r="B34">
         <v>517000</v>
       </c>
-      <c r="E36">
+      <c r="C34">
         <v>0.78</v>
       </c>
     </row>
-    <row r="37" spans="3:5">
-      <c r="C37" s="1">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
         <v>12389</v>
       </c>
-      <c r="D37">
+      <c r="B35">
         <v>520000</v>
       </c>
-      <c r="E37">
+      <c r="C35">
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="38" spans="3:5">
-      <c r="C38" s="1">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
         <v>12754</v>
       </c>
-      <c r="D38">
+      <c r="B36">
         <v>522000</v>
       </c>
-      <c r="E38">
+      <c r="C36">
         <v>0.38</v>
       </c>
     </row>
-    <row r="39" spans="3:5">
-      <c r="C39" s="1">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
         <v>13119</v>
       </c>
-      <c r="D39">
+      <c r="B37">
         <v>526000</v>
       </c>
-      <c r="E39">
+      <c r="C37">
         <v>0.77</v>
       </c>
     </row>
-    <row r="40" spans="3:5">
-      <c r="C40" s="1">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
         <v>13485</v>
       </c>
-      <c r="D40">
+      <c r="B38">
         <v>527000</v>
       </c>
-      <c r="E40">
+      <c r="C38">
         <v>0.19</v>
       </c>
     </row>
-    <row r="41" spans="3:5">
-      <c r="C41" s="1">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
         <v>13850</v>
       </c>
-      <c r="D41">
+      <c r="B39">
         <v>529000</v>
       </c>
-      <c r="E41">
+      <c r="C39">
         <v>0.38</v>
       </c>
     </row>
-    <row r="42" spans="3:5">
-      <c r="C42" s="1">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
         <v>14215</v>
       </c>
-      <c r="D42">
+      <c r="B40">
         <v>535000</v>
       </c>
-      <c r="E42">
+      <c r="C40">
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="43" spans="3:5">
-      <c r="C43" s="1">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
         <v>14580</v>
       </c>
-      <c r="D43">
+      <c r="B41">
         <v>543000</v>
       </c>
-      <c r="E43">
+      <c r="C41">
         <v>1.5</v>
       </c>
     </row>
-    <row r="44" spans="3:5">
-      <c r="C44" s="1">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
         <v>14946</v>
       </c>
-      <c r="D44">
+      <c r="B42">
         <v>552000</v>
       </c>
-      <c r="E44">
+      <c r="C42">
         <v>1.66</v>
       </c>
     </row>
-    <row r="45" spans="3:5">
-      <c r="C45" s="1">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
         <v>15311</v>
       </c>
-      <c r="D45">
+      <c r="B43">
         <v>551000</v>
       </c>
-      <c r="E45">
+      <c r="C43">
         <v>-0.18</v>
       </c>
     </row>
-    <row r="46" spans="3:5">
-      <c r="C46" s="1">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
         <v>15676</v>
       </c>
-      <c r="D46">
+      <c r="B44">
         <v>575000</v>
       </c>
-      <c r="E46">
+      <c r="C44">
         <v>4.3600000000000003</v>
       </c>
     </row>
-    <row r="47" spans="3:5">
-      <c r="C47" s="1">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
         <v>16041</v>
       </c>
-      <c r="D47">
+      <c r="B45">
         <v>631000</v>
       </c>
-      <c r="E47">
+      <c r="C45">
         <v>9.74</v>
       </c>
     </row>
-    <row r="48" spans="3:5">
-      <c r="C48" s="1">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
         <v>16407</v>
       </c>
-      <c r="D48">
+      <c r="B46">
         <v>605000</v>
       </c>
-      <c r="E48">
+      <c r="C46">
         <v>-4.12</v>
       </c>
     </row>
-    <row r="49" spans="3:5">
-      <c r="C49" s="1">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
         <v>16772</v>
       </c>
-      <c r="D49">
+      <c r="B47">
         <v>591000</v>
       </c>
-      <c r="E49">
+      <c r="C47">
         <v>-2.31</v>
       </c>
     </row>
-    <row r="50" spans="3:5">
-      <c r="C50" s="1">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
         <v>17137</v>
       </c>
-      <c r="D50">
+      <c r="B48">
         <v>638000</v>
       </c>
-      <c r="E50">
+      <c r="C48">
         <v>7.95</v>
       </c>
     </row>
-    <row r="51" spans="3:5">
-      <c r="C51" s="1">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
         <v>17502</v>
       </c>
-      <c r="D51">
+      <c r="B49">
         <v>636000</v>
       </c>
-      <c r="E51">
+      <c r="C49">
         <v>-0.31</v>
       </c>
     </row>
-    <row r="52" spans="3:5">
-      <c r="C52" s="1">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
         <v>17868</v>
       </c>
-      <c r="D52">
+      <c r="B50">
         <v>653000</v>
       </c>
-      <c r="E52">
+      <c r="C50">
         <v>2.67</v>
       </c>
     </row>
-    <row r="53" spans="3:5">
-      <c r="C53" s="1">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
         <v>18233</v>
       </c>
-      <c r="D53">
+      <c r="B51">
         <v>671000</v>
       </c>
-      <c r="E53">
+      <c r="C51">
         <v>2.76</v>
       </c>
     </row>
-    <row r="54" spans="3:5">
-      <c r="C54" s="1">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
         <v>18598</v>
       </c>
-      <c r="D54">
+      <c r="B52">
         <v>696000</v>
       </c>
-      <c r="E54">
+      <c r="C52">
         <v>3.73</v>
       </c>
     </row>
-    <row r="55" spans="3:5">
-      <c r="C55" s="1">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
         <v>18963</v>
       </c>
-      <c r="D55">
+      <c r="B53">
         <v>706000</v>
       </c>
-      <c r="E55">
+      <c r="C53">
         <v>1.44</v>
       </c>
     </row>
-    <row r="56" spans="3:5">
-      <c r="C56" s="1">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
         <v>19329</v>
       </c>
-      <c r="D56">
+      <c r="B54">
         <v>724000</v>
       </c>
-      <c r="E56">
+      <c r="C54">
         <v>2.5499999999999998</v>
       </c>
     </row>
-    <row r="57" spans="3:5">
-      <c r="C57" s="1">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
         <v>19694</v>
       </c>
-      <c r="D57">
+      <c r="B55">
         <v>739000</v>
       </c>
-      <c r="E57">
+      <c r="C55">
         <v>2.0699999999999998</v>
       </c>
     </row>
-    <row r="58" spans="3:5">
-      <c r="C58" s="1">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
         <v>20059</v>
       </c>
-      <c r="D58">
+      <c r="B56">
         <v>750000</v>
       </c>
-      <c r="E58">
+      <c r="C56">
         <v>1.49</v>
       </c>
     </row>
-    <row r="59" spans="3:5">
-      <c r="C59" s="1">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
         <v>20424</v>
       </c>
-      <c r="D59">
+      <c r="B57">
         <v>783000</v>
       </c>
-      <c r="E59">
+      <c r="C57">
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="60" spans="3:5">
-      <c r="C60" s="1">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
         <v>20790</v>
       </c>
-      <c r="D60">
+      <c r="B58">
         <v>809000</v>
       </c>
-      <c r="E60">
+      <c r="C58">
         <v>3.32</v>
       </c>
     </row>
-    <row r="61" spans="3:5">
-      <c r="C61" s="1">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
         <v>21155</v>
       </c>
-      <c r="D61">
+      <c r="B59">
         <v>826000</v>
       </c>
-      <c r="E61">
+      <c r="C59">
         <v>2.1</v>
       </c>
     </row>
-    <row r="62" spans="3:5">
-      <c r="C62" s="1">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
         <v>21520</v>
       </c>
-      <c r="D62">
+      <c r="B60">
         <v>845000</v>
       </c>
-      <c r="E62">
+      <c r="C60">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="63" spans="3:5">
-      <c r="C63" s="1">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
         <v>21885</v>
       </c>
-      <c r="D63">
+      <c r="B61">
         <v>870000</v>
       </c>
-      <c r="E63">
+      <c r="C61">
         <v>2.96</v>
       </c>
     </row>
-    <row r="64" spans="3:5">
-      <c r="C64" s="1">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
         <v>22251</v>
       </c>
-      <c r="D64">
+      <c r="B62">
         <v>900000</v>
       </c>
-      <c r="E64">
+      <c r="C62">
         <v>3.45</v>
       </c>
     </row>
-    <row r="65" spans="3:5">
-      <c r="C65" s="1">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
         <v>22616</v>
       </c>
-      <c r="D65">
+      <c r="B63">
         <v>936000</v>
       </c>
-      <c r="E65">
+      <c r="C63">
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="3:5">
-      <c r="C66" s="1">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
         <v>22981</v>
       </c>
-      <c r="D66">
+      <c r="B64">
         <v>958000</v>
       </c>
-      <c r="E66">
+      <c r="C64">
         <v>2.35</v>
       </c>
     </row>
-    <row r="67" spans="3:5">
-      <c r="C67" s="1">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
         <v>23346</v>
       </c>
-      <c r="D67">
+      <c r="B65">
         <v>974000</v>
       </c>
-      <c r="E67">
+      <c r="C65">
         <v>1.67</v>
       </c>
     </row>
-    <row r="68" spans="3:5">
-      <c r="C68" s="1">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
         <v>23712</v>
       </c>
-      <c r="D68">
+      <c r="B66">
         <v>978000</v>
       </c>
-      <c r="E68">
+      <c r="C66">
         <v>0.41</v>
       </c>
     </row>
-    <row r="69" spans="3:5">
-      <c r="C69" s="1">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
         <v>24077</v>
       </c>
-      <c r="D69">
+      <c r="B67">
         <v>994000</v>
       </c>
-      <c r="E69">
+      <c r="C67">
         <v>1.64</v>
       </c>
     </row>
-    <row r="70" spans="3:5">
-      <c r="C70" s="1">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
         <v>24442</v>
       </c>
-      <c r="D70">
+      <c r="B68">
         <v>1009000</v>
       </c>
-      <c r="E70">
+      <c r="C68">
         <v>1.51</v>
       </c>
     </row>
-    <row r="71" spans="3:5">
-      <c r="C71" s="1">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
         <v>24807</v>
       </c>
-      <c r="D71">
+      <c r="B69">
         <v>1019000</v>
       </c>
-      <c r="E71">
+      <c r="C69">
         <v>0.99</v>
       </c>
     </row>
-    <row r="72" spans="3:5">
-      <c r="C72" s="1">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
         <v>25173</v>
       </c>
-      <c r="D72">
+      <c r="B70">
         <v>1029000</v>
       </c>
-      <c r="E72">
+      <c r="C70">
         <v>0.98</v>
       </c>
     </row>
-    <row r="73" spans="3:5">
-      <c r="C73" s="1">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
         <v>25538</v>
       </c>
-      <c r="D73">
+      <c r="B71">
         <v>1047000</v>
       </c>
-      <c r="E73">
+      <c r="C71">
         <v>1.75</v>
       </c>
     </row>
-    <row r="74" spans="3:5">
-      <c r="C74" s="1">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
         <v>25903</v>
       </c>
-      <c r="D74">
+      <c r="B72">
         <v>1059273</v>
       </c>
-      <c r="E74">
+      <c r="C72">
         <v>1.17</v>
       </c>
     </row>
-    <row r="75" spans="3:5">
-      <c r="C75" s="1">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
         <v>26268</v>
       </c>
-      <c r="D75">
+      <c r="B73">
         <v>1101192</v>
       </c>
-      <c r="E75">
+      <c r="C73">
         <v>3.96</v>
       </c>
     </row>
-    <row r="76" spans="3:5">
-      <c r="C76" s="1">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
         <v>26634</v>
       </c>
-      <c r="D76">
+      <c r="B74">
         <v>1135449</v>
       </c>
-      <c r="E76">
+      <c r="C74">
         <v>3.11</v>
       </c>
     </row>
-    <row r="77" spans="3:5">
-      <c r="C77" s="1">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
         <v>26999</v>
       </c>
-      <c r="D77">
+      <c r="B75">
         <v>1170040</v>
       </c>
-      <c r="E77">
+      <c r="C75">
         <v>3.05</v>
       </c>
     </row>
-    <row r="78" spans="3:5">
-      <c r="C78" s="1">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
         <v>27364</v>
       </c>
-      <c r="D78">
+      <c r="B76">
         <v>1200471</v>
       </c>
-      <c r="E78">
+      <c r="C76">
         <v>2.6</v>
       </c>
     </row>
-    <row r="79" spans="3:5">
-      <c r="C79" s="1">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
         <v>27729</v>
       </c>
-      <c r="D79">
+      <c r="B77">
         <v>1236030</v>
       </c>
-      <c r="E79">
+      <c r="C77">
         <v>2.96</v>
       </c>
     </row>
-    <row r="80" spans="3:5">
-      <c r="C80" s="1">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
         <v>28095</v>
       </c>
-      <c r="D80">
+      <c r="B78">
         <v>1274928</v>
       </c>
-      <c r="E80">
+      <c r="C78">
         <v>3.15</v>
       </c>
     </row>
-    <row r="81" spans="3:5">
-      <c r="C81" s="1">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
         <v>28460</v>
       </c>
-      <c r="D81">
+      <c r="B79">
         <v>1319512</v>
       </c>
-      <c r="E81">
+      <c r="C79">
         <v>3.5</v>
       </c>
     </row>
-    <row r="82" spans="3:5">
-      <c r="C82" s="1">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
         <v>28825</v>
       </c>
-      <c r="D82">
+      <c r="B80">
         <v>1367510</v>
       </c>
-      <c r="E82">
+      <c r="C80">
         <v>3.64</v>
       </c>
     </row>
-    <row r="83" spans="3:5">
-      <c r="C83" s="1">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
         <v>29190</v>
       </c>
-      <c r="D83">
+      <c r="B81">
         <v>1420238</v>
       </c>
-      <c r="E83">
+      <c r="C81">
         <v>3.86</v>
       </c>
     </row>
-    <row r="84" spans="3:5">
-      <c r="C84" s="1">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
         <v>29556</v>
       </c>
-      <c r="D84">
+      <c r="B82">
         <v>1472595</v>
       </c>
-      <c r="E84">
+      <c r="C82">
         <v>3.69</v>
       </c>
     </row>
-    <row r="85" spans="3:5">
-      <c r="C85" s="1">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
         <v>29921</v>
       </c>
-      <c r="D85">
+      <c r="B83">
         <v>1515471</v>
       </c>
-      <c r="E85">
+      <c r="C83">
         <v>2.91</v>
       </c>
     </row>
-    <row r="86" spans="3:5">
-      <c r="C86" s="1">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
         <v>30286</v>
       </c>
-      <c r="D86">
+      <c r="B84">
         <v>1558314</v>
       </c>
-      <c r="E86">
+      <c r="C84">
         <v>2.83</v>
       </c>
     </row>
-    <row r="87" spans="3:5">
-      <c r="C87" s="1">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
         <v>30651</v>
       </c>
-      <c r="D87">
+      <c r="B85">
         <v>1594943</v>
       </c>
-      <c r="E87">
+      <c r="C85">
         <v>2.35</v>
       </c>
     </row>
-    <row r="88" spans="3:5">
-      <c r="C88" s="1">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
         <v>31017</v>
       </c>
-      <c r="D88">
+      <c r="B86">
         <v>1622342</v>
       </c>
-      <c r="E88">
+      <c r="C86">
         <v>1.72</v>
       </c>
     </row>
-    <row r="89" spans="3:5">
-      <c r="C89" s="1">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
         <v>31382</v>
       </c>
-      <c r="D89">
+      <c r="B87">
         <v>1642910</v>
       </c>
-      <c r="E89">
+      <c r="C87">
         <v>1.27</v>
       </c>
     </row>
-    <row r="90" spans="3:5">
-      <c r="C90" s="1">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
         <v>31747</v>
       </c>
-      <c r="D90">
+      <c r="B88">
         <v>1662834</v>
       </c>
-      <c r="E90">
+      <c r="C88">
         <v>1.21</v>
       </c>
     </row>
-    <row r="91" spans="3:5">
-      <c r="C91" s="1">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
         <v>32112</v>
       </c>
-      <c r="D91">
+      <c r="B89">
         <v>1678119</v>
       </c>
-      <c r="E91">
+      <c r="C89">
         <v>0.92</v>
       </c>
     </row>
-    <row r="92" spans="3:5">
-      <c r="C92" s="1">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
         <v>32478</v>
       </c>
-      <c r="D92">
+      <c r="B90">
         <v>1689372</v>
       </c>
-      <c r="E92">
+      <c r="C90">
         <v>0.67</v>
       </c>
     </row>
-    <row r="93" spans="3:5">
-      <c r="C93" s="1">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
         <v>32843</v>
       </c>
-      <c r="D93">
+      <c r="B91">
         <v>1705864</v>
       </c>
-      <c r="E93">
+      <c r="C91">
         <v>0.98</v>
       </c>
     </row>
-    <row r="94" spans="3:5">
-      <c r="C94" s="1">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
         <v>33208</v>
       </c>
-      <c r="D94">
+      <c r="B92">
         <v>1729722</v>
       </c>
-      <c r="E94">
+      <c r="C92">
         <v>1.4</v>
       </c>
     </row>
-    <row r="95" spans="3:5">
-      <c r="C95" s="1">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
         <v>33573</v>
       </c>
-      <c r="D95">
+      <c r="B93">
         <v>1771941</v>
       </c>
-      <c r="E95">
+      <c r="C93">
         <v>2.44</v>
       </c>
     </row>
-    <row r="96" spans="3:5">
-      <c r="C96" s="1">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
         <v>33939</v>
       </c>
-      <c r="D96">
+      <c r="B94">
         <v>1821498</v>
       </c>
-      <c r="E96">
+      <c r="C94">
         <v>2.8</v>
       </c>
     </row>
-    <row r="97" spans="3:5">
-      <c r="C97" s="1">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
         <v>34304</v>
       </c>
-      <c r="D97">
+      <c r="B95">
         <v>1875993</v>
       </c>
-      <c r="E97">
+      <c r="C95">
         <v>2.99</v>
       </c>
     </row>
-    <row r="98" spans="3:5">
-      <c r="C98" s="1">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
         <v>34669</v>
       </c>
-      <c r="D98">
+      <c r="B96">
         <v>1930436</v>
       </c>
-      <c r="E98">
+      <c r="C96">
         <v>2.9</v>
       </c>
     </row>
-    <row r="99" spans="3:5">
-      <c r="C99" s="1">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
         <v>35034</v>
       </c>
-      <c r="D99">
+      <c r="B97">
         <v>1976774</v>
       </c>
-      <c r="E99">
+      <c r="C97">
         <v>2.4</v>
       </c>
     </row>
-    <row r="100" spans="3:5">
-      <c r="C100" s="1">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
         <v>35400</v>
       </c>
-      <c r="D100">
+      <c r="B98">
         <v>2022253</v>
       </c>
-      <c r="E100">
+      <c r="C98">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="101" spans="3:5">
-      <c r="C101" s="1">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
         <v>35765</v>
       </c>
-      <c r="D101">
+      <c r="B99">
         <v>2065397</v>
       </c>
-      <c r="E101">
+      <c r="C99">
         <v>2.13</v>
       </c>
     </row>
-    <row r="102" spans="3:5">
-      <c r="C102" s="1">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
         <v>36130</v>
       </c>
-      <c r="D102">
+      <c r="B100">
         <v>2100562</v>
       </c>
-      <c r="E102">
+      <c r="C100">
         <v>1.7</v>
       </c>
     </row>
-    <row r="103" spans="3:5">
-      <c r="C103" s="1">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
         <v>36495</v>
       </c>
-      <c r="D103">
+      <c r="B101">
         <v>2129836</v>
       </c>
-      <c r="E103">
+      <c r="C101">
         <v>1.39</v>
       </c>
     </row>
-    <row r="104" spans="3:5">
-      <c r="C104" s="1">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="1">
         <v>36861</v>
       </c>
-      <c r="D104">
+      <c r="B102">
         <v>2244502</v>
       </c>
-      <c r="E104">
+      <c r="C102">
         <v>5.38</v>
       </c>
     </row>
-    <row r="105" spans="3:5">
-      <c r="C105" s="1">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
         <v>37226</v>
       </c>
-      <c r="D105">
+      <c r="B103">
         <v>2283715</v>
       </c>
-      <c r="E105">
+      <c r="C103">
         <v>1.75</v>
       </c>
     </row>
-    <row r="106" spans="3:5">
-      <c r="C106" s="1">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
         <v>37591</v>
       </c>
-      <c r="D106">
+      <c r="B104">
         <v>2324815</v>
       </c>
-      <c r="E106">
+      <c r="C104">
         <v>1.8</v>
       </c>
     </row>
-    <row r="107" spans="3:5">
-      <c r="C107" s="1">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
         <v>37956</v>
       </c>
-      <c r="D107">
+      <c r="B105">
         <v>2360137</v>
       </c>
-      <c r="E107">
+      <c r="C105">
         <v>1.52</v>
       </c>
     </row>
-    <row r="108" spans="3:5">
-      <c r="C108" s="1">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="1">
         <v>38322</v>
       </c>
-      <c r="D108">
+      <c r="B106">
         <v>2401580</v>
       </c>
-      <c r="E108">
+      <c r="C106">
         <v>1.76</v>
       </c>
     </row>
-    <row r="109" spans="3:5">
-      <c r="C109" s="1">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
         <v>38687</v>
       </c>
-      <c r="D109">
+      <c r="B107">
         <v>2457719</v>
       </c>
-      <c r="E109">
+      <c r="C107">
         <v>2.34</v>
       </c>
     </row>
-    <row r="110" spans="3:5">
-      <c r="C110" s="1">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
         <v>39052</v>
       </c>
-      <c r="D110">
+      <c r="B108">
         <v>2525507</v>
       </c>
-      <c r="E110">
+      <c r="C108">
         <v>2.76</v>
       </c>
     </row>
-    <row r="111" spans="3:5">
-      <c r="C111" s="1">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" s="1">
         <v>39417</v>
       </c>
-      <c r="D111">
+      <c r="B109">
         <v>2597746</v>
       </c>
-      <c r="E111">
+      <c r="C109">
         <v>2.86</v>
       </c>
     </row>
-    <row r="112" spans="3:5">
-      <c r="C112" s="1">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" s="1">
         <v>39783</v>
       </c>
-      <c r="D112">
+      <c r="B110">
         <v>2663029</v>
       </c>
-      <c r="E112">
+      <c r="C110">
         <v>2.5099999999999998</v>
       </c>
     </row>
-    <row r="113" spans="3:5">
-      <c r="C113" s="1">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" s="1">
         <v>40148</v>
       </c>
-      <c r="D113">
+      <c r="B111">
         <v>2723421</v>
       </c>
-      <c r="E113">
+      <c r="C111">
         <v>2.27</v>
       </c>
     </row>
-    <row r="114" spans="3:5">
-      <c r="C114" s="1">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" s="1">
         <v>40513</v>
       </c>
-      <c r="D114">
+      <c r="B112">
         <v>2775413</v>
       </c>
-      <c r="E114">
+      <c r="C112">
         <v>1.91</v>
       </c>
     </row>
-    <row r="115" spans="3:5">
-      <c r="C115" s="1">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" s="1">
         <v>40878</v>
       </c>
-      <c r="D115">
+      <c r="B113">
         <v>2814797</v>
       </c>
-      <c r="E115">
+      <c r="C113">
         <v>1.42</v>
       </c>
     </row>
-    <row r="116" spans="3:5">
-      <c r="C116" s="1">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" s="1">
         <v>41244</v>
       </c>
-      <c r="D116">
+      <c r="B114">
         <v>2854146</v>
       </c>
-      <c r="E116">
+      <c r="C114">
         <v>1.4</v>
       </c>
     </row>
-    <row r="117" spans="3:5">
-      <c r="C117" s="1">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" s="1">
         <v>41609</v>
       </c>
-      <c r="D117">
+      <c r="B115">
         <v>2898773</v>
       </c>
-      <c r="E117">
+      <c r="C115">
         <v>1.56</v>
       </c>
     </row>
-    <row r="118" spans="3:5">
-      <c r="C118" s="1">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" s="1">
         <v>41974</v>
       </c>
-      <c r="D118">
+      <c r="B116">
         <v>2938327</v>
       </c>
-      <c r="E118">
+      <c r="C116">
         <v>1.36</v>
       </c>
     </row>
-    <row r="119" spans="3:5">
-      <c r="C119" s="1">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" s="1">
         <v>42339</v>
       </c>
-      <c r="D119">
+      <c r="B117">
         <v>2983626</v>
       </c>
-      <c r="E119">
+      <c r="C117">
         <v>1.54</v>
       </c>
     </row>
-    <row r="120" spans="3:5">
-      <c r="C120" s="1">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" s="1">
         <v>42705</v>
       </c>
-      <c r="D120">
+      <c r="B118">
         <v>3044241</v>
       </c>
-      <c r="E120">
+      <c r="C118">
         <v>2.0299999999999998</v>
       </c>
     </row>
-    <row r="121" spans="3:5">
-      <c r="C121" s="1">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" s="1">
         <v>43070</v>
       </c>
-      <c r="D121">
+      <c r="B119">
         <v>3103540</v>
       </c>
-      <c r="E121">
+      <c r="C119">
         <v>1.95</v>
       </c>
     </row>
-    <row r="122" spans="3:5">
-      <c r="C122" s="1">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" s="1">
         <v>43435</v>
       </c>
-      <c r="D122">
+      <c r="B120">
         <v>3155153</v>
       </c>
-      <c r="E122">
+      <c r="C120">
         <v>1.66</v>
       </c>
     </row>
-    <row r="123" spans="3:5">
-      <c r="C123" s="1">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" s="1">
         <v>43800</v>
       </c>
-      <c r="D123">
+      <c r="B121">
         <v>3203383</v>
       </c>
-      <c r="E123">
+      <c r="C121">
         <v>1.53</v>
       </c>
     </row>
-    <row r="124" spans="3:5">
-      <c r="C124" s="1">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" s="1">
         <v>44166</v>
       </c>
-      <c r="D124">
+      <c r="B122">
         <v>3283785</v>
       </c>
-      <c r="E124">
+      <c r="C122">
         <v>2.5099999999999998</v>
       </c>
     </row>
-    <row r="125" spans="3:5">
-      <c r="C125" s="1">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" s="1">
         <v>44531</v>
       </c>
-      <c r="D125">
+      <c r="B123">
         <v>3339113</v>
       </c>
-      <c r="E125">
+      <c r="C123">
         <v>1.68</v>
       </c>
     </row>
-    <row r="126" spans="3:5">
-      <c r="C126" s="1">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" s="1">
         <v>44896</v>
       </c>
-      <c r="D126">
+      <c r="B124">
         <v>3380800</v>
       </c>
-      <c r="E126">
+      <c r="C124">
         <v>1.25</v>
       </c>
     </row>

</xml_diff>